<commit_message>
changement pour la mise en ligne
</commit_message>
<xml_diff>
--- a/uploads/creatXl.xlsx
+++ b/uploads/creatXl.xlsx
@@ -56,10 +56,10 @@
     <t>Yoann</t>
   </si>
   <si>
-    <t>La Descente des Alpes - M1</t>
-  </si>
-  <si>
-    <t>2021-02-27</t>
+    <t>soleil</t>
+  </si>
+  <si>
+    <t>2021-03-02</t>
   </si>
   <si>
     <t>M1</t>
@@ -497,7 +497,7 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -523,7 +523,7 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -549,7 +549,7 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -575,7 +575,7 @@
         <v>21</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -601,7 +601,7 @@
         <v>23</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -627,7 +627,7 @@
         <v>25</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -653,7 +653,7 @@
         <v>27</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -679,7 +679,7 @@
         <v>29</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>

</xml_diff>